<commit_message>
Atualizada Tabela de Consumo
</commit_message>
<xml_diff>
--- a/ConsumoCond.xlsx
+++ b/ConsumoCond.xlsx
@@ -14,12 +14,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Plan1!$A$1:$R$25</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="14">
   <si>
     <t>Sabesp</t>
   </si>
@@ -843,11 +843,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="66728448"/>
-        <c:axId val="112724800"/>
+        <c:axId val="219664384"/>
+        <c:axId val="162048832"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="66728448"/>
+        <c:axId val="219664384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -874,14 +874,14 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="112724800"/>
+        <c:crossAx val="162048832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="112724800"/>
+        <c:axId val="162048832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="360"/>
@@ -935,7 +935,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66728448"/>
+        <c:crossAx val="219664384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="20"/>
@@ -1317,10 +1317,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F221"/>
+  <dimension ref="A1:F245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
-      <selection activeCell="C222" sqref="C222"/>
+    <sheetView tabSelected="1" topLeftCell="A218" workbookViewId="0">
+      <selection activeCell="C221" sqref="C221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3979,6 +3979,270 @@
       </c>
       <c r="C221" s="28">
         <v>645</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A222" s="27">
+        <v>45352</v>
+      </c>
+      <c r="B222" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C222" s="28">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A223" s="27">
+        <v>45352</v>
+      </c>
+      <c r="B223" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C223" s="28">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A224" s="27">
+        <v>45383</v>
+      </c>
+      <c r="B224" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C224" s="31">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A225" s="27">
+        <v>45383</v>
+      </c>
+      <c r="B225" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C225" s="31">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A226" s="27">
+        <v>45413</v>
+      </c>
+      <c r="B226" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C226" s="31">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A227" s="27">
+        <v>45413</v>
+      </c>
+      <c r="B227" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C227" s="31">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A228" s="27">
+        <v>45444</v>
+      </c>
+      <c r="B228" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C228" s="31">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A229" s="27">
+        <v>45444</v>
+      </c>
+      <c r="B229" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C229" s="31">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A230" s="27">
+        <v>45474</v>
+      </c>
+      <c r="B230" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C230" s="31">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A231" s="27">
+        <v>45474</v>
+      </c>
+      <c r="B231" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C231" s="31">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A232" s="27">
+        <v>45505</v>
+      </c>
+      <c r="B232" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C232" s="31">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A233" s="27">
+        <v>45505</v>
+      </c>
+      <c r="B233" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C233" s="31">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A234" s="27">
+        <v>45536</v>
+      </c>
+      <c r="B234" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C234" s="31">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A235" s="27">
+        <v>45536</v>
+      </c>
+      <c r="B235" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C235" s="31">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A236" s="27">
+        <v>45566</v>
+      </c>
+      <c r="B236" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C236" s="31">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A237" s="27">
+        <v>45566</v>
+      </c>
+      <c r="B237" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C237" s="31">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A238" s="27">
+        <v>45597</v>
+      </c>
+      <c r="B238" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C238" s="31">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A239" s="27">
+        <v>45597</v>
+      </c>
+      <c r="B239" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C239" s="31">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A240" s="27">
+        <v>45627</v>
+      </c>
+      <c r="B240" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C240" s="31">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A241" s="27">
+        <v>45627</v>
+      </c>
+      <c r="B241" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C241" s="31">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A242" s="27">
+        <v>45658</v>
+      </c>
+      <c r="B242" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C242" s="31">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A243" s="27">
+        <v>45658</v>
+      </c>
+      <c r="B243" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C243" s="31">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A244" s="27">
+        <v>45689</v>
+      </c>
+      <c r="B244" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C244" s="31">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A245" s="27">
+        <v>45689</v>
+      </c>
+      <c r="B245" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C245" s="31">
+        <v>558</v>
       </c>
     </row>
   </sheetData>

</xml_diff>